<commit_message>
Changes in Output Results
</commit_message>
<xml_diff>
--- a/uploads/SEALIST_2324.xlsx
+++ b/uploads/SEALIST_2324.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1a4b8616e385e7b5/Desktop/RetentionGuard_UI/uploads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="26" documentId="8_{4271B4A6-ABAA-4F26-811A-46D9B7F58994}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5E125A06-4F86-4ACE-91A6-EDF4A9E6824B}"/>
+  <xr:revisionPtr revIDLastSave="34" documentId="8_{4271B4A6-ABAA-4F26-811A-46D9B7F58994}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4E92A11A-08FB-4EB9-BF10-6698BCFF31F7}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9DB15D10-55CD-46F8-8952-A54CEC7A2B5B}"/>
   </bookViews>
@@ -3304,7 +3304,7 @@
   <dimension ref="A1:N914"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>